<commit_message>
Added feature which gets discrete channel from ADC values
</commit_message>
<xml_diff>
--- a/Tables/Histogram_delimiters.xlsx
+++ b/Tables/Histogram_delimiters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Documents/MultiGrid/MultiGridMux/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF7CF7DF-61A6-C647-9515-B4FBBEAFF722}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336B4AE6-689D-A848-9F92-620CD894FDDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="2440" windowWidth="24140" windowHeight="17060" xr2:uid="{B3541E74-35F6-8141-BE24-EB4F0D049E16}"/>
+    <workbookView xWindow="14720" yWindow="2860" windowWidth="14340" windowHeight="17060" xr2:uid="{B3541E74-35F6-8141-BE24-EB4F0D049E16}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
-    <t>Wire Separation</t>
+    <t>Wires</t>
   </si>
   <si>
-    <t>Grid Separation</t>
+    <t>Grids</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Stop</t>
   </si>
 </sst>
 </file>
@@ -66,8 +72,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,94 +394,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15AD5837-A3B5-DE42-BEEF-269D4FD9C5CE}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" customWidth="1"/>
     <col min="11" max="11" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>450</v>
-      </c>
-      <c r="B2">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>445</v>
+      </c>
+      <c r="B3">
         <v>775</v>
       </c>
-      <c r="B3">
+      <c r="C3">
+        <v>870</v>
+      </c>
+      <c r="D3">
+        <v>1125</v>
+      </c>
+      <c r="G3">
+        <v>525</v>
+      </c>
+      <c r="H3">
         <v>780</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1100</v>
+        <v>780</v>
       </c>
       <c r="B4">
-        <v>1110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1417</v>
+        <v>1120</v>
       </c>
       <c r="B5">
-        <v>1430</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1765</v>
+        <v>1457</v>
       </c>
       <c r="B6">
-        <v>1776</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2090</v>
+        <v>1810</v>
       </c>
       <c r="B7">
-        <v>2118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>2420</v>
-      </c>
-      <c r="B8">
-        <v>2452</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>2755</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>3080</v>
+        <v>2150</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
help message and new channel order
</commit_message>
<xml_diff>
--- a/Tables/Histogram_delimiters.xlsx
+++ b/Tables/Histogram_delimiters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Documents/MultiGrid/MultiGridMux/Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabellejohn/Documents/MultiGridMUX/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CD4DA8-6326-F949-AFFC-BE83B9B212FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434FE5E7-37EA-7948-9CEE-19D9CB5FAE3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5720" yWindow="440" windowWidth="14340" windowHeight="16280" xr2:uid="{B3541E74-35F6-8141-BE24-EB4F0D049E16}"/>
+    <workbookView xWindow="11020" yWindow="500" windowWidth="14340" windowHeight="14480" xr2:uid="{B3541E74-35F6-8141-BE24-EB4F0D049E16}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -433,16 +433,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>445</v>
+        <v>465</v>
       </c>
       <c r="B3">
-        <v>775</v>
+        <v>805</v>
       </c>
       <c r="C3">
-        <v>870</v>
+        <v>905</v>
       </c>
       <c r="D3">
-        <v>1125</v>
+        <v>1160</v>
       </c>
       <c r="G3">
         <v>525</v>
@@ -453,34 +453,34 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>780</v>
+        <v>818</v>
       </c>
       <c r="B4">
-        <v>1120</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1120</v>
+        <v>1176</v>
       </c>
       <c r="B5">
-        <v>1457</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1457</v>
+        <v>1516</v>
       </c>
       <c r="B6">
-        <v>1805</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1810</v>
+        <v>1888</v>
       </c>
       <c r="B7">
-        <v>2150</v>
+        <v>2233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed plotting, and mapping
</commit_message>
<xml_diff>
--- a/Tables/Histogram_delimiters.xlsx
+++ b/Tables/Histogram_delimiters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabellejohn/Documents/MultiGridMUX/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BDEA66-EB48-9344-B496-7EEDD5F0580A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B53F038-80C3-014B-B19C-9829284B13E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="11260" yWindow="460" windowWidth="14340" windowHeight="14480" xr2:uid="{B3541E74-35F6-8141-BE24-EB4F0D049E16}"/>
+    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="13980" xr2:uid="{0204D40D-CD5E-7F48-BB1B-916F17CC27F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>Stop</t>
-  </si>
-  <si>
     <t>Wires  20x4</t>
   </si>
   <si>
@@ -43,6 +37,12 @@
   </si>
   <si>
     <t>Grids 1</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Stop</t>
   </si>
 </sst>
 </file>
@@ -81,10 +81,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -399,67 +399,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15AD5837-A3B5-DE42-BEEF-269D4FD9C5CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BEF214D-5184-6F40-903F-A04666B60090}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="21.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>1</v>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="B3">
         <v>805</v>
@@ -471,16 +466,16 @@
         <v>1160</v>
       </c>
       <c r="E3">
-        <v>467</v>
+        <v>456</v>
       </c>
       <c r="F3">
-        <v>799</v>
+        <v>803</v>
       </c>
       <c r="G3">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="H3">
-        <v>792</v>
+        <v>796</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -488,49 +483,49 @@
         <v>818</v>
       </c>
       <c r="B4">
-        <v>1153</v>
+        <v>1157</v>
       </c>
       <c r="E4">
-        <v>827</v>
+        <v>822</v>
       </c>
       <c r="F4">
-        <v>1159</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="B5">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="E5">
-        <v>1178</v>
+        <v>1175</v>
       </c>
       <c r="F5">
-        <v>1508</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1516</v>
+        <v>1520</v>
       </c>
       <c r="B6">
-        <v>1871</v>
+        <v>1873</v>
       </c>
       <c r="E6">
-        <v>1535</v>
+        <v>1529</v>
       </c>
       <c r="F6">
-        <v>1881</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1888</v>
+        <v>1889</v>
       </c>
       <c r="B7">
-        <v>2233</v>
+        <v>2232</v>
       </c>
     </row>
   </sheetData>
@@ -541,6 +536,5 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>